<commit_message>
Foi adicionado o sistema de inserção de dados junto ao excel substituindo o txt
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DERMO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Pecas</t>
+          <t>Pecas.AC</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -478,126 +478,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">04-07-2023 </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$3000.00 </t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$3000.00 </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$2000.00 </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$2000.00 </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  10Un </t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  -R$1000.00 </t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 66.67%</t>
-        </is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">31/03/2020 </t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$3000.00 </t>
+          <t>1000.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$6000.00 </t>
+          <t>3000.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$3000.00 </t>
+          <t>1000.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$5000.00 </t>
+          <t>2000.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  30Un </t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  -R$1000.00 </t>
+          <t>1000.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 83.33%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">04-07-2023 </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$6000.00 </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$12000.00 </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$5000.00 </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$10000.00 </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  70Un </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  -R$2000.00 </t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 83.33%</t>
+          <t>66.67</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foi feito o sistema de apagar lista junto ao excel, substituindo txt.
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,76 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2000.00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>66.67</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Testando o sistema implementado
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,132 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>40</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8000.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>7000.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>50.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sistema de inclusão e exclusão utilizando excel e as três listas funcionando corretamente
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,123 +481,39 @@
           <t>07/07/2023</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>40</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H4" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8000.00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7000.00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>50.0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>87.50</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>100.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foi realizado testes de aplicação com a nova estrutura de edição de dados, a estrutura parece estar solida, porém ainda não está implementada com o POO e o front-end, será implementado ainda nessa semana
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,48 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>10.0</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi implementado o sistema de edição selecionável em todas as listas
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,174 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>31/03/2001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3000.00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3000.00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3000.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3000.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/07/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4000.00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7000.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4000.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7000.00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>08/07/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8000.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>8000.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>08/07/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4000.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12000.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>9000.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3000.00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Após alguns testes na parte de editar as listas foi encontrado alguns problemas durante a execução, a maioria foi arrumado porém podem haver mais problemas, é necessário depurar constantemente fazendo diferentes testes
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,168 +478,448 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>31/03/2001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
+          <t>50/50/6000</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>08/07/2023</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4000.00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>7000.00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4000.00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7000.00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>08/07/2023</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>8000.00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>8000.00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>17000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>113.33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>08/07/2023</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4000.00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>12000.00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>9000.00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>3000.00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>75.00</t>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>25000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>29000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>70</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>80</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>116.67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>80/90/8000</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>780</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>114.29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>50/80/5000</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>500.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>35500.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>45000.00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>830</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>9500.00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>126.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>40500.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>51000.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>840.0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>10500.00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>125.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>45500.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>57000.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>850.0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>11500.00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>125.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>50500.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>63000.00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>860.0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>12500.00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>124.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>55500.00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>69000.00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>870.0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>13500.00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>124.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>10/10/5000</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>60500.00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6000.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>75000.00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>880.0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>14500.00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>123.97</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agora quando o usuário editar um valor os inputs serão limpos, os inputs de inserção de valores agora não aceitaram mais valores negativos
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -677,40 +677,26 @@
           <t>50/80/5000</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>500.00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>35500.00</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>45000.00</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>830</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>9500.00</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>126.76</t>
-        </is>
+      <c r="B9" t="n">
+        <v>500</v>
+      </c>
+      <c r="C9" t="n">
+        <v>35500</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>45000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>830</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9500</v>
+      </c>
+      <c r="H9" t="n">
+        <v>126.76</v>
       </c>
     </row>
     <row r="10">
@@ -719,40 +705,26 @@
           <t>10/10/5000</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>40500.00</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>51000.00</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>840.0</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>10500.00</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>125.93</t>
-        </is>
+      <c r="B10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>40500</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>51000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>840</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10500</v>
+      </c>
+      <c r="H10" t="n">
+        <v>125.93</v>
       </c>
     </row>
     <row r="11">
@@ -761,40 +733,26 @@
           <t>10/10/5000</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>45500.00</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>57000.00</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>850.0</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>11500.00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>125.27</t>
-        </is>
+      <c r="B11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>45500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>57000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>850</v>
+      </c>
+      <c r="G11" t="n">
+        <v>11500</v>
+      </c>
+      <c r="H11" t="n">
+        <v>125.27</v>
       </c>
     </row>
     <row r="12">
@@ -803,40 +761,26 @@
           <t>10/10/5000</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>50500.00</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>63000.00</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>860.0</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>12500.00</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>124.75</t>
-        </is>
+      <c r="B12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50500</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>63000</v>
+      </c>
+      <c r="F12" t="n">
+        <v>860</v>
+      </c>
+      <c r="G12" t="n">
+        <v>12500</v>
+      </c>
+      <c r="H12" t="n">
+        <v>124.75</v>
       </c>
     </row>
     <row r="13">
@@ -845,40 +789,26 @@
           <t>10/10/5000</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>55500.00</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>69000.00</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>870.0</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>13500.00</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>124.32</t>
-        </is>
+      <c r="B13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>55500</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>69000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>870</v>
+      </c>
+      <c r="G13" t="n">
+        <v>13500</v>
+      </c>
+      <c r="H13" t="n">
+        <v>124.32</v>
       </c>
     </row>
     <row r="14">
@@ -887,39 +817,67 @@
           <t>10/10/5000</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>60500.00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6000.00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>75000.00</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>880.0</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>14500.00</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>123.97</t>
+      <c r="B14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>60500</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>75000</v>
+      </c>
+      <c r="F14" t="n">
+        <v>880</v>
+      </c>
+      <c r="G14" t="n">
+        <v>14500</v>
+      </c>
+      <c r="H14" t="n">
+        <v>123.97</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>50/84/9000</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7847.00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>68347.00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7417.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>82417.00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>897.0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>14070.00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>120.59</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foi feito a formatação dos backups, agora tem 'R$' e também identifica quando não bater as metas o sinal de menos '-' atrás do valor junto com o 'R$'.
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,132 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>14/07/2023</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>14/07/2023</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>109.09</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>14/07/2023</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>14/07/2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>21000.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>7000.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>21000.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>40.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
As fontes foram ajustadas conforme o necessário para android/desktop
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,23 +478,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>14/07/2023</t>
+          <t>30/05/2000</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="C2" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="D2" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="E2" t="n">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -506,126 +506,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>14/07/2023</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>11000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H3" t="n">
-        <v>109.09</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>14/07/2023</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>16000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="H4" t="n">
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>14/07/2023</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C5" t="n">
-        <v>21000</v>
-      </c>
-      <c r="D5" t="n">
-        <v>7000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>21000</v>
-      </c>
-      <c r="F5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>08/08/2001</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6000.90</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>27000.90</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>5226.03</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>26226.03</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>72.0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>774.87</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>97.13</t>
+          <t>31/07/2000</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1000.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>100.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foram ajustados os tamanhos dos popups para android e as fontes fora da tela
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,76 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>30/05/2000</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>31/07/2000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
As classes foram devidamente separadas
</commit_message>
<xml_diff>
--- a/storage/listaDERMO.xlsx
+++ b/storage/listaDERMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,39 +509,123 @@
           <t>12/05/2000</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2525.00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>7535.00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2412.40</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6626.40</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>54.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>2525</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7535</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2412.4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6626.4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>54</v>
+      </c>
+      <c r="G3" t="n">
+        <v>908.6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>87.94</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>31/35/5000</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12535</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11626.4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>74</v>
+      </c>
+      <c r="G4" t="n">
+        <v>908.6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>92.75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>31/06/2000</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14535</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13626.4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>94</v>
+      </c>
+      <c r="G5" t="n">
+        <v>908.6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20/08/8000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8000.00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>22535.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>8000.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>21626.40</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>144.0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>908.60</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>87.94</t>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>95.97</t>
         </is>
       </c>
     </row>

</xml_diff>